<commit_message>
init dandelion spread algorithm.
</commit_message>
<xml_diff>
--- a/src/Output/result.xlsx
+++ b/src/Output/result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\2023HiMCM\src\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568BC854-0558-45C4-A28D-19D9D849A773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD27FE1-AFA3-46C4-8B84-2056D39D70F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="692">
   <si>
     <t>locality</t>
   </si>
@@ -2090,13 +2090,23 @@
   </si>
   <si>
     <t>https://plants.usda.gov/home/plantProfile?symbol=ZOMA2</t>
+  </si>
+  <si>
+    <t>Taraxacum officinale ssp. officinale</t>
+  </si>
+  <si>
+    <t>Common dandelion</t>
+  </si>
+  <si>
+    <t>https://plants.usda.gov/home/plantProfile?symbol=TAOF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2114,6 +2124,14 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2149,16 +2167,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2459,10 +2485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G226"/>
+  <dimension ref="A1:G227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -7674,9 +7701,35 @@
         <v>688</v>
       </c>
     </row>
+    <row r="227" spans="1:7">
+      <c r="A227" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="D227" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E227" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F227" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G227" s="3" t="s">
+        <v>691</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G226" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G227" r:id="rId1" xr:uid="{7F2FB057-A045-4970-A79F-E421F4C7D418}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>